<commit_message>
updated bug#1 with screenshots
</commit_message>
<xml_diff>
--- a/Bug.xlsx
+++ b/Bug.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\Desktop\Level-4\Capstone\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishali\PycharmProjects\Convolutional-neural-network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C8A6F1-A9E7-4290-92D1-5352E1A6FFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA23A9C-5ACC-4FEF-BC4B-12CE873B9612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E26622D4-E653-48DB-9F60-66DD60752617}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug#1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Bug ID#1</t>
   </si>
@@ -69,6 +70,9 @@
   </si>
   <si>
     <t>Yeman</t>
+  </si>
+  <si>
+    <t>From below picture the empty values diplay as NaN which is not valid add in the code will reduce performance</t>
   </si>
 </sst>
 </file>
@@ -118,10 +122,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,6 +144,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>443157</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>30974</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC9999B0-380A-F8C0-DB52-14BAFF5F7635}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2011680"/>
+          <a:ext cx="13808637" cy="5700254"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1661438</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>30625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33263C80-3BAB-3035-6097-5FD8BB456B54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8412480"/>
+          <a:ext cx="3208298" cy="1676545"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,13 +559,13 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="53.77734375" customWidth="1"/>
+    <col min="2" max="2" width="74.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -495,7 +595,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
@@ -517,5 +620,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16FEA2D-9D6C-4740-8356-03E3FC2E8477}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>